<commit_message>
Finished c and c++ version (multithreaded), trying to find upper limit for prolog (single thread)
</commit_message>
<xml_diff>
--- a/Project/results.xlsx
+++ b/Project/results.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>C</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Processes</t>
   </si>
@@ -29,6 +26,12 @@
   </si>
   <si>
     <t>Execution time (s)</t>
+  </si>
+  <si>
+    <t>C, primes until 1750, upper limit: 2^1000000</t>
+  </si>
+  <si>
+    <t>C++, primes until 1750, upper limit: 2^1000000</t>
   </si>
 </sst>
 </file>
@@ -373,165 +376,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>263.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>195.26</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>332.596</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>347.62</v>
+        <v>244.2</v>
       </c>
       <c r="C4">
         <f>B3/B4</f>
-        <v>0.7593061388872907</v>
+        <v>0.79959049959049955</v>
       </c>
       <c r="D4">
         <f>C4/A4</f>
-        <v>0.37965306944364535</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.39979524979524977</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>215.13900000000001</v>
+      </c>
+      <c r="H4">
+        <f>G3/G4</f>
+        <v>1.5459586592853922</v>
+      </c>
+      <c r="I4">
+        <f>H4/F4</f>
+        <v>0.77297932964269611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>411.76</v>
+        <v>291.37</v>
       </c>
       <c r="C5">
         <f>B3/B5</f>
-        <v>0.64102875461433839</v>
+        <v>0.67014448982393515</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D10" si="0">C5/A5</f>
-        <v>0.21367625153811279</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.22338149660797837</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>201.66</v>
+      </c>
+      <c r="H5">
+        <f>G3/G5</f>
+        <v>1.6492908856491124</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I10" si="1">H5/F5</f>
+        <v>0.54976362854970418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>441.2</v>
+        <v>369.59</v>
       </c>
       <c r="C6">
         <f>B3/B6</f>
-        <v>0.59825475974614684</v>
+        <v>0.52831516004220891</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.14956368993653671</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.13207879001055223</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>189.02600000000001</v>
+      </c>
+      <c r="H6">
+        <f>G3/G6</f>
+        <v>1.7595251446890903</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0.43988128617227257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>424.56</v>
+        <v>364.32</v>
       </c>
       <c r="C7">
         <f>B3/B7</f>
-        <v>0.62170246843791221</v>
+        <v>0.53595740008783488</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.12434049368758245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.10719148001756698</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>186.32</v>
+      </c>
+      <c r="H7">
+        <f>G3/G7</f>
+        <v>1.7850794332331474</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0.35701588664662948</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>449.43</v>
+        <v>376.23</v>
       </c>
       <c r="C8">
         <f>B3/B8</f>
-        <v>0.58729946821529488</v>
+        <v>0.51899104271323393</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>9.7883244702549152E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8.6498507118872317E-2</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>184.761</v>
+      </c>
+      <c r="H8">
+        <f>G3/G8</f>
+        <v>1.8001418048181164</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.30002363413635275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>449.2</v>
+        <v>395.68</v>
       </c>
       <c r="C9">
         <f>B3/B9</f>
-        <v>0.58760017809439002</v>
+        <v>0.49347957945814797</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>8.3942882584912865E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7.0497082779735418E-2</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>188.00800000000001</v>
+      </c>
+      <c r="H9">
+        <f>G3/G9</f>
+        <v>1.7690523807497553</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.25272176867853646</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>450.48</v>
+        <v>388.31</v>
       </c>
       <c r="C10">
         <f>B3/B10</f>
-        <v>0.58593056295507007</v>
+        <v>0.50284566454636759</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>7.3241320369383758E-2</v>
+        <v>6.2855708068295948E-2</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>183.37200000000001</v>
+      </c>
+      <c r="H10">
+        <f>G3/G10</f>
+        <v>1.8137774578452543</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.22672218223065679</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added results for openMP
</commit_message>
<xml_diff>
--- a/Project/results.xlsx
+++ b/Project/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Processes</t>
   </si>
@@ -31,7 +31,10 @@
     <t>C, primes until 1750, upper limit: 2^1000000</t>
   </si>
   <si>
-    <t>C++, primes until 1750, upper limit: 2^1000000</t>
+    <t>OpenMP, primes until 1750, upper limit: 2^1000000</t>
+  </si>
+  <si>
+    <t>C++, primes until 2000, upper limit: 2^1000000</t>
   </si>
 </sst>
 </file>
@@ -67,10 +70,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +406,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -656,10 +662,153 @@
         <v>0.22672218223065679</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>194.28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>202.59</v>
+      </c>
+      <c r="C15">
+        <f>B14/B15</f>
+        <v>0.95898119354361022</v>
+      </c>
+      <c r="D15">
+        <f>C15/A15</f>
+        <v>0.47949059677180511</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>217.84</v>
+      </c>
+      <c r="C16">
+        <f>B14/B16</f>
+        <v>0.89184722732280575</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D21" si="2">C16/A16</f>
+        <v>0.2972824091076019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>231.65</v>
+      </c>
+      <c r="C17">
+        <f>B14/B17</f>
+        <v>0.83867904165767315</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.20966976041441829</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>247.35</v>
+      </c>
+      <c r="C18">
+        <f>B14/B18</f>
+        <v>0.78544572468162521</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0.15708914493632503</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>281.20999999999998</v>
+      </c>
+      <c r="C19">
+        <f>B14/B19</f>
+        <v>0.6908715906262225</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>0.11514526510437041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>298.5</v>
+      </c>
+      <c r="C20">
+        <f>B14/B20</f>
+        <v>0.65085427135678398</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>9.2979181622397711E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>305.33999999999997</v>
+      </c>
+      <c r="C21">
+        <f>B14/B21</f>
+        <v>0.63627431715464733</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>7.9534289644330916E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added results for prolog
</commit_message>
<xml_diff>
--- a/Project/results.xlsx
+++ b/Project/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Processes</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>C++, primes until 2000, upper limit: 2^1000000</t>
+  </si>
+  <si>
+    <t>Prolog, primes until 10000, upper limit: 2^1000000</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,6 +672,12 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -683,6 +692,18 @@
       <c r="D13" t="s">
         <v>2</v>
       </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -691,6 +712,12 @@
       <c r="B14">
         <v>194.28</v>
       </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>283.81</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -707,6 +734,20 @@
         <f>C15/A15</f>
         <v>0.47949059677180511</v>
       </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>178.55</v>
+      </c>
+      <c r="H15">
+        <f>G14/G15</f>
+        <v>1.5895267432091851</v>
+      </c>
+      <c r="I15">
+        <f>H15/F15</f>
+        <v>0.79476337160459254</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -723,8 +764,22 @@
         <f t="shared" ref="D16:D21" si="2">C16/A16</f>
         <v>0.2972824091076019</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>153</v>
+      </c>
+      <c r="H16">
+        <f>G14/G16</f>
+        <v>1.8549673202614378</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16:I21" si="3">H16/F16</f>
+        <v>0.61832244008714599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -739,8 +794,22 @@
         <f t="shared" si="2"/>
         <v>0.20966976041441829</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>151.28</v>
+      </c>
+      <c r="H17">
+        <f>G14/G17</f>
+        <v>1.8760576414595451</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>0.46901441036488628</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -755,8 +824,22 @@
         <f t="shared" si="2"/>
         <v>0.15708914493632503</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>150.56</v>
+      </c>
+      <c r="H18">
+        <f>G14/G18</f>
+        <v>1.885029224229543</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>0.3770058448459086</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -771,8 +854,22 @@
         <f t="shared" si="2"/>
         <v>0.11514526510437041</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>151.19</v>
+      </c>
+      <c r="H19">
+        <f>G14/G19</f>
+        <v>1.8771744162973742</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>0.31286240271622906</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -787,8 +884,22 @@
         <f t="shared" si="2"/>
         <v>9.2979181622397711E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>150.63</v>
+      </c>
+      <c r="H20">
+        <f>G14/G20</f>
+        <v>1.8841532231295228</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>0.26916474616136038</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -803,12 +914,27 @@
         <f t="shared" si="2"/>
         <v>7.9534289644330916E-2</v>
       </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <v>151.03</v>
+      </c>
+      <c r="H21">
+        <f>G14/G21</f>
+        <v>1.8791630801827452</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>0.23489538502284316</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>